<commit_message>
Tests added & scrapping perfomrance improved
</commit_message>
<xml_diff>
--- a/general_bond_data.xlsx
+++ b/general_bond_data.xlsx
@@ -653,7 +653,7 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -877,7 +877,7 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -989,7 +989,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -2893,7 +2893,7 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -3229,7 +3229,7 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -3565,7 +3565,7 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -4349,7 +4349,7 @@
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -4685,7 +4685,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -4797,7 +4797,7 @@
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -4909,7 +4909,7 @@
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -5021,7 +5021,7 @@
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -5245,7 +5245,7 @@
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -5581,7 +5581,7 @@
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -5693,7 +5693,7 @@
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -5805,7 +5805,7 @@
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -6029,7 +6029,7 @@
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -6253,7 +6253,7 @@
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -6365,7 +6365,7 @@
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -6477,7 +6477,7 @@
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -6589,7 +6589,7 @@
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -6813,7 +6813,7 @@
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -6925,7 +6925,7 @@
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -7037,7 +7037,7 @@
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -7149,7 +7149,7 @@
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -7261,7 +7261,7 @@
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -7373,7 +7373,7 @@
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -7485,7 +7485,7 @@
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -7597,7 +7597,7 @@
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -7709,7 +7709,7 @@
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -7821,7 +7821,7 @@
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -7933,7 +7933,7 @@
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -8045,7 +8045,7 @@
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -8157,7 +8157,7 @@
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -8269,7 +8269,7 @@
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -8381,7 +8381,7 @@
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -8493,7 +8493,7 @@
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -8605,7 +8605,7 @@
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -8717,7 +8717,7 @@
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -8829,7 +8829,7 @@
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -8941,7 +8941,7 @@
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -9053,7 +9053,7 @@
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -9165,7 +9165,7 @@
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -9277,7 +9277,7 @@
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -9389,7 +9389,7 @@
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -9501,7 +9501,7 @@
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -9613,7 +9613,7 @@
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -9725,7 +9725,7 @@
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -9837,7 +9837,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -9949,7 +9949,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -10061,7 +10061,7 @@
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -10173,7 +10173,7 @@
       </c>
       <c r="V87" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -10285,7 +10285,7 @@
       </c>
       <c r="V88" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -10397,7 +10397,7 @@
       </c>
       <c r="V89" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -10509,7 +10509,7 @@
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -10621,7 +10621,7 @@
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -10733,7 +10733,7 @@
       </c>
       <c r="V92" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -10845,7 +10845,7 @@
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -10957,7 +10957,7 @@
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -11069,7 +11069,7 @@
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -11181,7 +11181,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -11293,7 +11293,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -11405,7 +11405,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -11517,7 +11517,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -11629,7 +11629,7 @@
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -11741,7 +11741,7 @@
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -11853,7 +11853,7 @@
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -11965,7 +11965,7 @@
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -12077,7 +12077,7 @@
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -12189,7 +12189,7 @@
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -12301,7 +12301,7 @@
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -12413,7 +12413,7 @@
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -12525,7 +12525,7 @@
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -12637,7 +12637,7 @@
       </c>
       <c r="V109" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -12749,7 +12749,7 @@
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -12861,7 +12861,7 @@
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -12973,7 +12973,7 @@
       </c>
       <c r="V112" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -13085,7 +13085,7 @@
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -13197,7 +13197,7 @@
       </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -13309,7 +13309,7 @@
       </c>
       <c r="V115" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -13421,7 +13421,7 @@
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -13533,7 +13533,7 @@
       </c>
       <c r="V117" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -13645,7 +13645,7 @@
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -13757,7 +13757,7 @@
       </c>
       <c r="V119" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -13869,7 +13869,7 @@
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -13981,7 +13981,7 @@
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -14093,7 +14093,7 @@
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -14205,7 +14205,7 @@
       </c>
       <c r="V123" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -14317,7 +14317,7 @@
       </c>
       <c r="V124" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -14429,7 +14429,7 @@
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -14541,7 +14541,7 @@
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -14653,7 +14653,7 @@
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -14765,7 +14765,7 @@
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -14877,7 +14877,7 @@
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -14989,7 +14989,7 @@
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -15101,7 +15101,7 @@
       </c>
       <c r="V131" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -15213,7 +15213,7 @@
       </c>
       <c r="V132" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -15325,7 +15325,7 @@
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -15437,7 +15437,7 @@
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -15549,7 +15549,7 @@
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -15661,7 +15661,7 @@
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -15773,7 +15773,7 @@
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -15885,7 +15885,7 @@
       </c>
       <c r="V138" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -15997,7 +15997,7 @@
       </c>
       <c r="V139" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -16109,7 +16109,7 @@
       </c>
       <c r="V140" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -16221,7 +16221,7 @@
       </c>
       <c r="V141" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -16333,7 +16333,7 @@
       </c>
       <c r="V142" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -16445,7 +16445,7 @@
       </c>
       <c r="V143" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -16557,7 +16557,7 @@
       </c>
       <c r="V144" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -16669,7 +16669,7 @@
       </c>
       <c r="V145" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -16781,7 +16781,7 @@
       </c>
       <c r="V146" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -16893,7 +16893,7 @@
       </c>
       <c r="V147" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -17005,7 +17005,7 @@
       </c>
       <c r="V148" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -17117,7 +17117,7 @@
       </c>
       <c r="V149" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -17229,7 +17229,7 @@
       </c>
       <c r="V150" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -17341,7 +17341,7 @@
       </c>
       <c r="V151" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -17453,7 +17453,7 @@
       </c>
       <c r="V152" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -17565,7 +17565,7 @@
       </c>
       <c r="V153" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -17677,7 +17677,7 @@
       </c>
       <c r="V154" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -17789,7 +17789,7 @@
       </c>
       <c r="V155" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -17901,7 +17901,7 @@
       </c>
       <c r="V156" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -18013,7 +18013,7 @@
       </c>
       <c r="V157" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -18125,7 +18125,7 @@
       </c>
       <c r="V158" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -18237,7 +18237,7 @@
       </c>
       <c r="V159" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -18349,7 +18349,7 @@
       </c>
       <c r="V160" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -18461,7 +18461,7 @@
       </c>
       <c r="V161" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -18573,7 +18573,7 @@
       </c>
       <c r="V162" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -18685,7 +18685,7 @@
       </c>
       <c r="V163" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -18797,7 +18797,7 @@
       </c>
       <c r="V164" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -18909,7 +18909,7 @@
       </c>
       <c r="V165" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -19021,7 +19021,7 @@
       </c>
       <c r="V166" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -19133,7 +19133,7 @@
       </c>
       <c r="V167" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -19245,7 +19245,7 @@
       </c>
       <c r="V168" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -19357,7 +19357,7 @@
       </c>
       <c r="V169" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -19469,7 +19469,7 @@
       </c>
       <c r="V170" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -19581,7 +19581,7 @@
       </c>
       <c r="V171" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -19693,7 +19693,7 @@
       </c>
       <c r="V172" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -19805,7 +19805,7 @@
       </c>
       <c r="V173" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -19917,7 +19917,7 @@
       </c>
       <c r="V174" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -20029,7 +20029,7 @@
       </c>
       <c r="V175" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -20141,7 +20141,7 @@
       </c>
       <c r="V176" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -20253,7 +20253,7 @@
       </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -20365,7 +20365,7 @@
       </c>
       <c r="V178" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -20477,7 +20477,7 @@
       </c>
       <c r="V179" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -20589,7 +20589,7 @@
       </c>
       <c r="V180" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -20701,7 +20701,7 @@
       </c>
       <c r="V181" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -20813,7 +20813,7 @@
       </c>
       <c r="V182" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -20925,7 +20925,7 @@
       </c>
       <c r="V183" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -21037,7 +21037,7 @@
       </c>
       <c r="V184" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -21149,7 +21149,7 @@
       </c>
       <c r="V185" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -21261,7 +21261,7 @@
       </c>
       <c r="V186" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -21373,7 +21373,7 @@
       </c>
       <c r="V187" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -21485,7 +21485,7 @@
       </c>
       <c r="V188" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -21597,7 +21597,7 @@
       </c>
       <c r="V189" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -21709,7 +21709,7 @@
       </c>
       <c r="V190" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -21821,7 +21821,7 @@
       </c>
       <c r="V191" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -21933,7 +21933,7 @@
       </c>
       <c r="V192" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -22045,7 +22045,7 @@
       </c>
       <c r="V193" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -22157,7 +22157,7 @@
       </c>
       <c r="V194" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -22269,7 +22269,7 @@
       </c>
       <c r="V195" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -22381,7 +22381,7 @@
       </c>
       <c r="V196" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -22493,7 +22493,7 @@
       </c>
       <c r="V197" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -22605,7 +22605,7 @@
       </c>
       <c r="V198" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -22717,7 +22717,7 @@
       </c>
       <c r="V199" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -22829,7 +22829,7 @@
       </c>
       <c r="V200" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -22941,7 +22941,7 @@
       </c>
       <c r="V201" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -23053,7 +23053,7 @@
       </c>
       <c r="V202" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -23165,7 +23165,7 @@
       </c>
       <c r="V203" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -23277,7 +23277,7 @@
       </c>
       <c r="V204" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -23389,7 +23389,7 @@
       </c>
       <c r="V205" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -23501,7 +23501,7 @@
       </c>
       <c r="V206" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -23613,7 +23613,7 @@
       </c>
       <c r="V207" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -23725,7 +23725,7 @@
       </c>
       <c r="V208" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -23837,7 +23837,7 @@
       </c>
       <c r="V209" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -23949,7 +23949,7 @@
       </c>
       <c r="V210" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -24061,7 +24061,7 @@
       </c>
       <c r="V211" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -24173,7 +24173,7 @@
       </c>
       <c r="V212" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -24285,7 +24285,7 @@
       </c>
       <c r="V213" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -24397,7 +24397,7 @@
       </c>
       <c r="V214" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -24509,7 +24509,7 @@
       </c>
       <c r="V215" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -24621,7 +24621,7 @@
       </c>
       <c r="V216" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -24733,7 +24733,7 @@
       </c>
       <c r="V217" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -24845,7 +24845,7 @@
       </c>
       <c r="V218" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -24957,7 +24957,7 @@
       </c>
       <c r="V219" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -25069,7 +25069,7 @@
       </c>
       <c r="V220" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -25181,7 +25181,7 @@
       </c>
       <c r="V221" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -25293,7 +25293,7 @@
       </c>
       <c r="V222" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -25405,7 +25405,7 @@
       </c>
       <c r="V223" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -25517,7 +25517,7 @@
       </c>
       <c r="V224" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -25629,7 +25629,7 @@
       </c>
       <c r="V225" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -25741,7 +25741,7 @@
       </c>
       <c r="V226" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -25853,7 +25853,7 @@
       </c>
       <c r="V227" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -25965,7 +25965,7 @@
       </c>
       <c r="V228" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -26077,7 +26077,7 @@
       </c>
       <c r="V229" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -26189,7 +26189,7 @@
       </c>
       <c r="V230" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -26301,7 +26301,7 @@
       </c>
       <c r="V231" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -26413,7 +26413,7 @@
       </c>
       <c r="V232" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -26525,7 +26525,7 @@
       </c>
       <c r="V233" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -26637,7 +26637,7 @@
       </c>
       <c r="V234" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -26749,7 +26749,7 @@
       </c>
       <c r="V235" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -26861,7 +26861,7 @@
       </c>
       <c r="V236" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -26973,7 +26973,7 @@
       </c>
       <c r="V237" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -27085,7 +27085,7 @@
       </c>
       <c r="V238" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -27197,7 +27197,7 @@
       </c>
       <c r="V239" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -27309,7 +27309,7 @@
       </c>
       <c r="V240" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -27421,7 +27421,7 @@
       </c>
       <c r="V241" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -27533,7 +27533,7 @@
       </c>
       <c r="V242" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -27645,7 +27645,7 @@
       </c>
       <c r="V243" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -27757,7 +27757,7 @@
       </c>
       <c r="V244" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -27869,7 +27869,7 @@
       </c>
       <c r="V245" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -27981,7 +27981,7 @@
       </c>
       <c r="V246" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -28093,7 +28093,7 @@
       </c>
       <c r="V247" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -28205,7 +28205,7 @@
       </c>
       <c r="V248" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -28317,7 +28317,7 @@
       </c>
       <c r="V249" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -28429,7 +28429,7 @@
       </c>
       <c r="V250" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -28541,7 +28541,7 @@
       </c>
       <c r="V251" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -28653,7 +28653,7 @@
       </c>
       <c r="V252" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -28765,7 +28765,7 @@
       </c>
       <c r="V253" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -28877,7 +28877,7 @@
       </c>
       <c r="V254" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -28989,7 +28989,7 @@
       </c>
       <c r="V255" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -29101,7 +29101,7 @@
       </c>
       <c r="V256" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -29213,7 +29213,7 @@
       </c>
       <c r="V257" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -29325,7 +29325,7 @@
       </c>
       <c r="V258" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -29437,7 +29437,7 @@
       </c>
       <c r="V259" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -29549,7 +29549,7 @@
       </c>
       <c r="V260" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -29661,7 +29661,7 @@
       </c>
       <c r="V261" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -29773,7 +29773,7 @@
       </c>
       <c r="V262" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -29885,7 +29885,7 @@
       </c>
       <c r="V263" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -29997,7 +29997,7 @@
       </c>
       <c r="V264" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -30109,7 +30109,7 @@
       </c>
       <c r="V265" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -30221,7 +30221,7 @@
       </c>
       <c r="V266" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -30333,7 +30333,7 @@
       </c>
       <c r="V267" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -30445,7 +30445,7 @@
       </c>
       <c r="V268" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -30557,7 +30557,7 @@
       </c>
       <c r="V269" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -30669,7 +30669,7 @@
       </c>
       <c r="V270" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -30781,7 +30781,7 @@
       </c>
       <c r="V271" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -30893,7 +30893,7 @@
       </c>
       <c r="V272" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -31005,7 +31005,7 @@
       </c>
       <c r="V273" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -31117,7 +31117,7 @@
       </c>
       <c r="V274" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -31229,7 +31229,7 @@
       </c>
       <c r="V275" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -31341,7 +31341,7 @@
       </c>
       <c r="V276" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -31453,7 +31453,7 @@
       </c>
       <c r="V277" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -31565,7 +31565,7 @@
       </c>
       <c r="V278" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -31677,7 +31677,7 @@
       </c>
       <c r="V279" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>
@@ -31789,7 +31789,7 @@
       </c>
       <c r="V280" t="inlineStr">
         <is>
-          <t>2025-01-05 20:55:25</t>
+          <t>2025-01-05 22:42:05</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
theme details updated, scrapping floats improved, bondportfolio added new methods, added new analysis to app.py
</commit_message>
<xml_diff>
--- a/general_bond_data.xlsx
+++ b/general_bond_data.xlsx
@@ -653,7 +653,7 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -877,7 +877,7 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -989,7 +989,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -2893,7 +2893,7 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -3229,7 +3229,7 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -3565,7 +3565,7 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4125,7 @@
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -4349,7 +4349,7 @@
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="V36" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -4685,7 +4685,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -4797,7 +4797,7 @@
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -4909,7 +4909,7 @@
       </c>
       <c r="V40" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -5021,7 +5021,7 @@
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -5245,7 +5245,7 @@
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -5581,7 +5581,7 @@
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -5693,7 +5693,7 @@
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -5805,7 +5805,7 @@
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -6029,7 +6029,7 @@
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -6253,7 +6253,7 @@
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -6365,7 +6365,7 @@
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -6477,7 +6477,7 @@
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -6589,7 +6589,7 @@
       </c>
       <c r="V55" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -6813,7 +6813,7 @@
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -6925,7 +6925,7 @@
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -7037,7 +7037,7 @@
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -7149,7 +7149,7 @@
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -7261,7 +7261,7 @@
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -7373,7 +7373,7 @@
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -7485,7 +7485,7 @@
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -7597,7 +7597,7 @@
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -7709,7 +7709,7 @@
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -7821,7 +7821,7 @@
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -7933,7 +7933,7 @@
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -8045,7 +8045,7 @@
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -8157,7 +8157,7 @@
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -8269,7 +8269,7 @@
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -8381,7 +8381,7 @@
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -8493,7 +8493,7 @@
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -8605,7 +8605,7 @@
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -8717,7 +8717,7 @@
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -8829,7 +8829,7 @@
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -8941,7 +8941,7 @@
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -9053,7 +9053,7 @@
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -9165,7 +9165,7 @@
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -9277,7 +9277,7 @@
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -9389,7 +9389,7 @@
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -9501,7 +9501,7 @@
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -9613,7 +9613,7 @@
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -9725,7 +9725,7 @@
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -9837,7 +9837,7 @@
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -9949,7 +9949,7 @@
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -10061,7 +10061,7 @@
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -10173,7 +10173,7 @@
       </c>
       <c r="V87" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -10285,7 +10285,7 @@
       </c>
       <c r="V88" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -10397,7 +10397,7 @@
       </c>
       <c r="V89" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -10509,7 +10509,7 @@
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -10621,7 +10621,7 @@
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -10733,7 +10733,7 @@
       </c>
       <c r="V92" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -10845,7 +10845,7 @@
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -10957,7 +10957,7 @@
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -11069,7 +11069,7 @@
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -11181,7 +11181,7 @@
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -11293,7 +11293,7 @@
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -11405,7 +11405,7 @@
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -11517,7 +11517,7 @@
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -11629,7 +11629,7 @@
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -11741,7 +11741,7 @@
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -11853,7 +11853,7 @@
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -11965,7 +11965,7 @@
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -12077,7 +12077,7 @@
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -12189,7 +12189,7 @@
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -12301,7 +12301,7 @@
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -12413,7 +12413,7 @@
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -12525,7 +12525,7 @@
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -12637,7 +12637,7 @@
       </c>
       <c r="V109" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -12749,7 +12749,7 @@
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -12861,7 +12861,7 @@
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -12973,7 +12973,7 @@
       </c>
       <c r="V112" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -13085,7 +13085,7 @@
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -13197,7 +13197,7 @@
       </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -13309,7 +13309,7 @@
       </c>
       <c r="V115" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -13421,7 +13421,7 @@
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -13533,7 +13533,7 @@
       </c>
       <c r="V117" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -13645,7 +13645,7 @@
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -13757,7 +13757,7 @@
       </c>
       <c r="V119" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -13869,7 +13869,7 @@
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -13981,7 +13981,7 @@
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -14093,7 +14093,7 @@
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -14205,7 +14205,7 @@
       </c>
       <c r="V123" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -14317,7 +14317,7 @@
       </c>
       <c r="V124" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -14429,7 +14429,7 @@
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -14541,7 +14541,7 @@
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -14653,7 +14653,7 @@
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -14765,7 +14765,7 @@
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -14877,7 +14877,7 @@
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -14989,7 +14989,7 @@
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -15101,7 +15101,7 @@
       </c>
       <c r="V131" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -15213,7 +15213,7 @@
       </c>
       <c r="V132" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -15325,7 +15325,7 @@
       </c>
       <c r="V133" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -15437,7 +15437,7 @@
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -15549,7 +15549,7 @@
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -15661,7 +15661,7 @@
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -15773,7 +15773,7 @@
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -15885,7 +15885,7 @@
       </c>
       <c r="V138" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -15997,7 +15997,7 @@
       </c>
       <c r="V139" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -16109,7 +16109,7 @@
       </c>
       <c r="V140" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -16221,7 +16221,7 @@
       </c>
       <c r="V141" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -16333,7 +16333,7 @@
       </c>
       <c r="V142" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -16445,7 +16445,7 @@
       </c>
       <c r="V143" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -16557,7 +16557,7 @@
       </c>
       <c r="V144" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -16669,7 +16669,7 @@
       </c>
       <c r="V145" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -16781,7 +16781,7 @@
       </c>
       <c r="V146" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -16893,7 +16893,7 @@
       </c>
       <c r="V147" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -17005,7 +17005,7 @@
       </c>
       <c r="V148" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -17117,7 +17117,7 @@
       </c>
       <c r="V149" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -17229,7 +17229,7 @@
       </c>
       <c r="V150" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -17341,7 +17341,7 @@
       </c>
       <c r="V151" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -17453,7 +17453,7 @@
       </c>
       <c r="V152" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -17565,7 +17565,7 @@
       </c>
       <c r="V153" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -17677,7 +17677,7 @@
       </c>
       <c r="V154" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -17789,7 +17789,7 @@
       </c>
       <c r="V155" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -17901,7 +17901,7 @@
       </c>
       <c r="V156" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -18013,7 +18013,7 @@
       </c>
       <c r="V157" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -18125,7 +18125,7 @@
       </c>
       <c r="V158" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -18237,7 +18237,7 @@
       </c>
       <c r="V159" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -18349,7 +18349,7 @@
       </c>
       <c r="V160" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -18461,7 +18461,7 @@
       </c>
       <c r="V161" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -18573,7 +18573,7 @@
       </c>
       <c r="V162" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -18685,7 +18685,7 @@
       </c>
       <c r="V163" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -18797,7 +18797,7 @@
       </c>
       <c r="V164" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -18909,7 +18909,7 @@
       </c>
       <c r="V165" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -19021,7 +19021,7 @@
       </c>
       <c r="V166" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -19133,7 +19133,7 @@
       </c>
       <c r="V167" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -19245,7 +19245,7 @@
       </c>
       <c r="V168" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -19357,7 +19357,7 @@
       </c>
       <c r="V169" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -19469,7 +19469,7 @@
       </c>
       <c r="V170" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -19581,7 +19581,7 @@
       </c>
       <c r="V171" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -19693,7 +19693,7 @@
       </c>
       <c r="V172" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -19805,7 +19805,7 @@
       </c>
       <c r="V173" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -19917,7 +19917,7 @@
       </c>
       <c r="V174" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -20029,7 +20029,7 @@
       </c>
       <c r="V175" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -20141,7 +20141,7 @@
       </c>
       <c r="V176" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -20253,7 +20253,7 @@
       </c>
       <c r="V177" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -20365,7 +20365,7 @@
       </c>
       <c r="V178" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -20477,7 +20477,7 @@
       </c>
       <c r="V179" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -20589,7 +20589,7 @@
       </c>
       <c r="V180" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -20701,7 +20701,7 @@
       </c>
       <c r="V181" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -20813,7 +20813,7 @@
       </c>
       <c r="V182" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -20925,7 +20925,7 @@
       </c>
       <c r="V183" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -21037,7 +21037,7 @@
       </c>
       <c r="V184" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -21149,7 +21149,7 @@
       </c>
       <c r="V185" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -21261,7 +21261,7 @@
       </c>
       <c r="V186" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -21373,7 +21373,7 @@
       </c>
       <c r="V187" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -21485,7 +21485,7 @@
       </c>
       <c r="V188" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -21597,7 +21597,7 @@
       </c>
       <c r="V189" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -21709,7 +21709,7 @@
       </c>
       <c r="V190" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -21821,7 +21821,7 @@
       </c>
       <c r="V191" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -21933,7 +21933,7 @@
       </c>
       <c r="V192" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -22045,7 +22045,7 @@
       </c>
       <c r="V193" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -22157,7 +22157,7 @@
       </c>
       <c r="V194" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -22269,7 +22269,7 @@
       </c>
       <c r="V195" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -22381,7 +22381,7 @@
       </c>
       <c r="V196" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -22493,7 +22493,7 @@
       </c>
       <c r="V197" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -22605,7 +22605,7 @@
       </c>
       <c r="V198" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -22717,7 +22717,7 @@
       </c>
       <c r="V199" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -22829,7 +22829,7 @@
       </c>
       <c r="V200" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -22941,7 +22941,7 @@
       </c>
       <c r="V201" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -23053,7 +23053,7 @@
       </c>
       <c r="V202" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -23165,7 +23165,7 @@
       </c>
       <c r="V203" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -23277,7 +23277,7 @@
       </c>
       <c r="V204" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -23389,7 +23389,7 @@
       </c>
       <c r="V205" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -23501,7 +23501,7 @@
       </c>
       <c r="V206" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -23613,7 +23613,7 @@
       </c>
       <c r="V207" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -23725,7 +23725,7 @@
       </c>
       <c r="V208" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -23837,7 +23837,7 @@
       </c>
       <c r="V209" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -23949,7 +23949,7 @@
       </c>
       <c r="V210" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -24061,7 +24061,7 @@
       </c>
       <c r="V211" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -24173,7 +24173,7 @@
       </c>
       <c r="V212" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -24285,7 +24285,7 @@
       </c>
       <c r="V213" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -24397,7 +24397,7 @@
       </c>
       <c r="V214" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -24509,7 +24509,7 @@
       </c>
       <c r="V215" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -24621,7 +24621,7 @@
       </c>
       <c r="V216" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -24733,7 +24733,7 @@
       </c>
       <c r="V217" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -24845,7 +24845,7 @@
       </c>
       <c r="V218" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -24957,7 +24957,7 @@
       </c>
       <c r="V219" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -25069,7 +25069,7 @@
       </c>
       <c r="V220" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -25181,7 +25181,7 @@
       </c>
       <c r="V221" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -25293,7 +25293,7 @@
       </c>
       <c r="V222" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -25405,7 +25405,7 @@
       </c>
       <c r="V223" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -25517,7 +25517,7 @@
       </c>
       <c r="V224" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -25629,7 +25629,7 @@
       </c>
       <c r="V225" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -25741,7 +25741,7 @@
       </c>
       <c r="V226" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -25853,7 +25853,7 @@
       </c>
       <c r="V227" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -25965,7 +25965,7 @@
       </c>
       <c r="V228" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -26077,7 +26077,7 @@
       </c>
       <c r="V229" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -26189,7 +26189,7 @@
       </c>
       <c r="V230" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -26301,7 +26301,7 @@
       </c>
       <c r="V231" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -26413,7 +26413,7 @@
       </c>
       <c r="V232" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -26525,7 +26525,7 @@
       </c>
       <c r="V233" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -26637,7 +26637,7 @@
       </c>
       <c r="V234" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -26749,7 +26749,7 @@
       </c>
       <c r="V235" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -26861,7 +26861,7 @@
       </c>
       <c r="V236" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -26973,7 +26973,7 @@
       </c>
       <c r="V237" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -27085,7 +27085,7 @@
       </c>
       <c r="V238" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -27197,7 +27197,7 @@
       </c>
       <c r="V239" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -27309,7 +27309,7 @@
       </c>
       <c r="V240" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -27421,7 +27421,7 @@
       </c>
       <c r="V241" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -27533,7 +27533,7 @@
       </c>
       <c r="V242" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -27645,7 +27645,7 @@
       </c>
       <c r="V243" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -27757,7 +27757,7 @@
       </c>
       <c r="V244" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -27869,7 +27869,7 @@
       </c>
       <c r="V245" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -27981,7 +27981,7 @@
       </c>
       <c r="V246" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -28093,7 +28093,7 @@
       </c>
       <c r="V247" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -28205,7 +28205,7 @@
       </c>
       <c r="V248" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -28317,7 +28317,7 @@
       </c>
       <c r="V249" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -28429,7 +28429,7 @@
       </c>
       <c r="V250" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -28541,7 +28541,7 @@
       </c>
       <c r="V251" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -28653,7 +28653,7 @@
       </c>
       <c r="V252" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -28765,7 +28765,7 @@
       </c>
       <c r="V253" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -28877,7 +28877,7 @@
       </c>
       <c r="V254" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -28989,7 +28989,7 @@
       </c>
       <c r="V255" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -29101,7 +29101,7 @@
       </c>
       <c r="V256" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -29213,7 +29213,7 @@
       </c>
       <c r="V257" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -29325,7 +29325,7 @@
       </c>
       <c r="V258" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -29437,7 +29437,7 @@
       </c>
       <c r="V259" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -29549,7 +29549,7 @@
       </c>
       <c r="V260" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -29661,7 +29661,7 @@
       </c>
       <c r="V261" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -29773,7 +29773,7 @@
       </c>
       <c r="V262" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -29885,7 +29885,7 @@
       </c>
       <c r="V263" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -29997,7 +29997,7 @@
       </c>
       <c r="V264" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -30109,7 +30109,7 @@
       </c>
       <c r="V265" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -30221,7 +30221,7 @@
       </c>
       <c r="V266" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -30333,7 +30333,7 @@
       </c>
       <c r="V267" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -30445,7 +30445,7 @@
       </c>
       <c r="V268" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -30557,7 +30557,7 @@
       </c>
       <c r="V269" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -30669,7 +30669,7 @@
       </c>
       <c r="V270" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -30781,7 +30781,7 @@
       </c>
       <c r="V271" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -30893,7 +30893,7 @@
       </c>
       <c r="V272" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -31005,7 +31005,7 @@
       </c>
       <c r="V273" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -31117,7 +31117,7 @@
       </c>
       <c r="V274" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -31229,7 +31229,7 @@
       </c>
       <c r="V275" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -31341,7 +31341,7 @@
       </c>
       <c r="V276" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -31453,7 +31453,7 @@
       </c>
       <c r="V277" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -31565,7 +31565,7 @@
       </c>
       <c r="V278" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -31677,7 +31677,7 @@
       </c>
       <c r="V279" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>
@@ -31789,7 +31789,7 @@
       </c>
       <c r="V280" t="inlineStr">
         <is>
-          <t>2025-01-05 22:42:05</t>
+          <t>2025-01-06 10:47:35</t>
         </is>
       </c>
     </row>

</xml_diff>